<commit_message>
integrated curtailment into power flow and fixed customer load profiles
</commit_message>
<xml_diff>
--- a/data/derived/res_bus/vm_pu.xlsx
+++ b/data/derived/res_bus/vm_pu.xlsx
@@ -481,100 +481,100 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.9987006308333087</v>
+        <v>0.9996016135675202</v>
       </c>
       <c r="D2">
-        <v>0.9945140798156457</v>
+        <v>0.9984268196153621</v>
       </c>
       <c r="E2">
-        <v>0.9967289058877395</v>
+        <v>0.9991238952742136</v>
       </c>
       <c r="F2">
+        <v>0.9999999999999998</v>
+      </c>
+      <c r="G2">
+        <v>0.9973751737279055</v>
+      </c>
+      <c r="H2">
+        <v>1.00008614505868</v>
+      </c>
+      <c r="I2">
+        <v>0.9966570219475814</v>
+      </c>
+      <c r="J2">
+        <v>0.9981877184263612</v>
+      </c>
+      <c r="K2">
+        <v>0.9999965045679907</v>
+      </c>
+      <c r="L2">
+        <v>0.9999655446517416</v>
+      </c>
+      <c r="M2">
         <v>0.9999999999999999</v>
       </c>
-      <c r="G2">
-        <v>0.9899743340206234</v>
-      </c>
-      <c r="H2">
-        <v>0.9974909634267954</v>
-      </c>
-      <c r="I2">
-        <v>0.9867101610977714</v>
-      </c>
-      <c r="J2">
-        <v>0.9921458250661074</v>
-      </c>
-      <c r="K2">
-        <v>0.9992646384570832</v>
-      </c>
-      <c r="L2">
-        <v>0.9994605616281186</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
       <c r="N2">
-        <v>0.993437868893752</v>
+        <v>0.9971752648869036</v>
       </c>
       <c r="O2">
-        <v>0.9905340815041079</v>
+        <v>0.9964004991558888</v>
       </c>
       <c r="P2">
-        <v>0.9892310779918829</v>
+        <v>0.9956933479933715</v>
       </c>
       <c r="Q2">
-        <v>0.9879678050920444</v>
+        <v>0.994977522528832</v>
       </c>
       <c r="R2">
-        <v>0.986097654303259</v>
+        <v>0.9940525156302441</v>
       </c>
       <c r="S2">
-        <v>0.9855361023983449</v>
+        <v>0.9937886786824849</v>
       </c>
       <c r="T2">
-        <v>0.997041812071739</v>
+        <v>0.9993743891020026</v>
       </c>
       <c r="U2">
-        <v>0.9922519195067013</v>
+        <v>0.9977185882150342</v>
       </c>
       <c r="V2">
-        <v>0.9912412937414319</v>
+        <v>0.997425587312049</v>
       </c>
       <c r="W2">
-        <v>0.9900727801110756</v>
+        <v>0.9971715100638725</v>
       </c>
       <c r="X2">
-        <v>0.9888599356738343</v>
+        <v>0.9967995142251189</v>
       </c>
       <c r="Y2">
-        <v>0.9780717191561961</v>
+        <v>0.9950721022767505</v>
       </c>
       <c r="Z2">
-        <v>0.9706363347428055</v>
+        <v>0.9948574034359604</v>
       </c>
       <c r="AA2">
-        <v>0.9874881950636795</v>
+        <v>0.9966723075176139</v>
       </c>
       <c r="AB2">
-        <v>0.9841382964949982</v>
+        <v>0.9957563601235208</v>
       </c>
       <c r="AC2">
-        <v>0.9698207744642318</v>
+        <v>0.9926016771325374</v>
       </c>
       <c r="AD2">
-        <v>0.9593975912978555</v>
+        <v>0.9905965209389909</v>
       </c>
       <c r="AE2">
-        <v>0.9543879015053018</v>
+        <v>0.9897383637730401</v>
       </c>
       <c r="AF2">
-        <v>0.9503768683465654</v>
+        <v>0.9886826691665317</v>
       </c>
       <c r="AG2">
-        <v>0.9494945260620397</v>
+        <v>0.9886091021207182</v>
       </c>
       <c r="AH2">
-        <v>0.949221424368591</v>
+        <v>0.9886099254707226</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -585,100 +585,100 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.9987263481757175</v>
+        <v>0.9996276968668369</v>
       </c>
       <c r="D3">
-        <v>0.994637136620548</v>
+        <v>0.9985293985378937</v>
       </c>
       <c r="E3">
-        <v>0.9967983176317589</v>
+        <v>0.9991818766246432</v>
       </c>
       <c r="F3">
-        <v>0.9999999999999998</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0.9900982464354333</v>
+        <v>0.9975394460543872</v>
       </c>
       <c r="H3">
-        <v>0.9974575933435699</v>
+        <v>1.000052192401207</v>
       </c>
       <c r="I3">
-        <v>0.9869232850721796</v>
+        <v>0.996888635802022</v>
       </c>
       <c r="J3">
-        <v>0.9922899824772872</v>
+        <v>0.9983125387003643</v>
       </c>
       <c r="K3">
-        <v>0.9992728884942943</v>
+        <v>0.9999928097693059</v>
       </c>
       <c r="L3">
-        <v>0.9994664856686424</v>
+        <v>0.9999652534808732</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
       <c r="N3">
-        <v>0.9935764306420746</v>
+        <v>0.9973527876444588</v>
       </c>
       <c r="O3">
-        <v>0.9907240404947755</v>
+        <v>0.9966274433895568</v>
       </c>
       <c r="P3">
-        <v>0.9894212911101937</v>
+        <v>0.9959651427360137</v>
       </c>
       <c r="Q3">
-        <v>0.9881582642582667</v>
+        <v>0.9952946129965708</v>
       </c>
       <c r="R3">
-        <v>0.986288478947309</v>
+        <v>0.9944283176351167</v>
       </c>
       <c r="S3">
-        <v>0.9857270361623205</v>
+        <v>0.994181126107256</v>
       </c>
       <c r="T3">
-        <v>0.9970760664371717</v>
+        <v>0.9994157130998982</v>
       </c>
       <c r="U3">
-        <v>0.9923592954686116</v>
+        <v>0.9978644137924462</v>
       </c>
       <c r="V3">
-        <v>0.9913680543968892</v>
+        <v>0.9975899211222941</v>
       </c>
       <c r="W3">
-        <v>0.9902329632703013</v>
+        <v>0.9973518624174669</v>
       </c>
       <c r="X3">
-        <v>0.9891177757985922</v>
+        <v>0.9970044409674196</v>
       </c>
       <c r="Y3">
-        <v>0.978597100714371</v>
+        <v>0.9953857721701734</v>
       </c>
       <c r="Z3">
-        <v>0.9714251061785453</v>
+        <v>0.9951846282110406</v>
       </c>
       <c r="AA3">
-        <v>0.9876530872843017</v>
+        <v>0.9968811473601377</v>
       </c>
       <c r="AB3">
-        <v>0.9843605594021994</v>
+        <v>0.9960232869361407</v>
       </c>
       <c r="AC3">
-        <v>0.9702594701101568</v>
+        <v>0.9930692524501477</v>
       </c>
       <c r="AD3">
-        <v>0.9600000859756755</v>
+        <v>0.9911914722244656</v>
       </c>
       <c r="AE3">
-        <v>0.9550925956214515</v>
+        <v>0.9903877168654807</v>
       </c>
       <c r="AF3">
-        <v>0.9510845634509805</v>
+        <v>0.9893992334283058</v>
       </c>
       <c r="AG3">
-        <v>0.9502028815529583</v>
+        <v>0.9893304225976749</v>
       </c>
       <c r="AH3">
-        <v>0.9499299847592333</v>
+        <v>0.9893312465484209</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -689,100 +689,100 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.9987400492391095</v>
+        <v>0.9996409182825959</v>
       </c>
       <c r="D4">
-        <v>0.9947018596998116</v>
+        <v>0.9985813720712404</v>
       </c>
       <c r="E4">
-        <v>0.9968356820138156</v>
+        <v>0.9992114356717228</v>
       </c>
       <c r="F4">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0.9901598173457211</v>
+        <v>0.9976211132385918</v>
       </c>
       <c r="H4">
-        <v>0.9974407724563051</v>
+        <v>1.000035063158959</v>
       </c>
       <c r="I4">
-        <v>0.9870290417673737</v>
+        <v>0.9970034503189509</v>
       </c>
       <c r="J4">
-        <v>0.9923614926786234</v>
+        <v>0.9983742486580589</v>
       </c>
       <c r="K4">
-        <v>0.9992768827416796</v>
+        <v>0.9999908009518577</v>
       </c>
       <c r="L4">
-        <v>0.9994693569444802</v>
+        <v>0.9999649958157876</v>
       </c>
       <c r="M4">
-        <v>0.9999999999999998</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0.9936456906333604</v>
+        <v>0.9974415081710259</v>
       </c>
       <c r="O4">
-        <v>0.9908189899132717</v>
+        <v>0.996740856013655</v>
       </c>
       <c r="P4">
-        <v>0.9895163675154494</v>
+        <v>0.996100965846716</v>
       </c>
       <c r="Q4">
-        <v>0.9882534636127922</v>
+        <v>0.9954530693495913</v>
       </c>
       <c r="R4">
-        <v>0.9863838609297386</v>
+        <v>0.9946161099391083</v>
       </c>
       <c r="S4">
-        <v>0.9858224726715347</v>
+        <v>0.9943772361018255</v>
       </c>
       <c r="T4">
-        <v>0.997094029938995</v>
+        <v>0.9994365426287553</v>
       </c>
       <c r="U4">
-        <v>0.9924138100990118</v>
+        <v>0.9979374768478776</v>
       </c>
       <c r="V4">
-        <v>0.99143225889915</v>
+        <v>0.9976722355868521</v>
       </c>
       <c r="W4">
-        <v>0.9903138751614271</v>
+        <v>0.9974421838461333</v>
       </c>
       <c r="X4">
-        <v>0.989249794259999</v>
+        <v>0.9971075647543249</v>
       </c>
       <c r="Y4">
-        <v>0.9788627092119845</v>
+        <v>0.995543239826815</v>
       </c>
       <c r="Z4">
-        <v>0.9718222530980047</v>
+        <v>0.995348870048007</v>
       </c>
       <c r="AA4">
-        <v>0.9877351175815124</v>
+        <v>0.9969850732756695</v>
       </c>
       <c r="AB4">
-        <v>0.9844712328376829</v>
+        <v>0.9961562225827361</v>
       </c>
       <c r="AC4">
-        <v>0.9704781903025399</v>
+        <v>0.9933023850027011</v>
       </c>
       <c r="AD4">
-        <v>0.9603005941537401</v>
+        <v>0.991488218764412</v>
       </c>
       <c r="AE4">
-        <v>0.9554441419491583</v>
+        <v>0.9907116339004339</v>
       </c>
       <c r="AF4">
-        <v>0.9514376051848977</v>
+        <v>0.9897567169576352</v>
       </c>
       <c r="AG4">
-        <v>0.9505562523603662</v>
+        <v>0.9896902815669983</v>
       </c>
       <c r="AH4">
-        <v>0.9502834576691375</v>
+        <v>0.9896911058174483</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -793,100 +793,100 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.9987540948070645</v>
+        <v>0.9996541867216798</v>
       </c>
       <c r="D5">
-        <v>0.9947678851896351</v>
+        <v>0.9986335275846137</v>
       </c>
       <c r="E5">
-        <v>0.9968741391231689</v>
+        <v>0.9992411503139366</v>
       </c>
       <c r="F5">
         <v>0.9999999999999999</v>
       </c>
       <c r="G5">
-        <v>0.9902211337167829</v>
+        <v>0.9977024707775224</v>
       </c>
       <c r="H5">
-        <v>0.9974238615992035</v>
+        <v>1.000017832747144</v>
       </c>
       <c r="I5">
-        <v>0.9871342674465881</v>
+        <v>0.99711761071177</v>
       </c>
       <c r="J5">
-        <v>0.9924326280834297</v>
+        <v>0.9984354971967379</v>
       </c>
       <c r="K5">
-        <v>0.9992807908022434</v>
+        <v>0.9999886857992295</v>
       </c>
       <c r="L5">
-        <v>0.9994721684155937</v>
+        <v>0.9999646643204827</v>
       </c>
       <c r="M5">
-        <v>0.9999999999999998</v>
+        <v>0.9999999999999997</v>
       </c>
       <c r="N5">
-        <v>0.9937149367136485</v>
+        <v>0.9975302014980474</v>
       </c>
       <c r="O5">
-        <v>0.9909139192967001</v>
+        <v>0.9968542290302794</v>
       </c>
       <c r="P5">
-        <v>0.9896114238343159</v>
+        <v>0.9962367395199727</v>
       </c>
       <c r="Q5">
-        <v>0.9883486428311882</v>
+        <v>0.9956114665337307</v>
       </c>
       <c r="R5">
-        <v>0.9864792227021064</v>
+        <v>0.9948038298840979</v>
       </c>
       <c r="S5">
-        <v>0.985917888948591</v>
+        <v>0.9945732703964134</v>
       </c>
       <c r="T5">
-        <v>0.9971123335160598</v>
+        <v>0.9994574110085767</v>
       </c>
       <c r="U5">
-        <v>0.9924686572480056</v>
+        <v>0.9980105671223108</v>
       </c>
       <c r="V5">
-        <v>0.9914967940332996</v>
+        <v>0.9977545754436307</v>
       </c>
       <c r="W5">
-        <v>0.9903951148286509</v>
+        <v>0.9975325291096959</v>
       </c>
       <c r="X5">
-        <v>0.9893830458593238</v>
+        <v>0.9972108542783417</v>
       </c>
       <c r="Y5">
-        <v>0.979129420670143</v>
+        <v>0.9957008542521629</v>
       </c>
       <c r="Z5">
-        <v>0.9722203917836492</v>
+        <v>0.9955132564176028</v>
       </c>
       <c r="AA5">
-        <v>0.9878168730830345</v>
+        <v>0.9970886729311614</v>
       </c>
       <c r="AB5">
-        <v>0.9845816034630755</v>
+        <v>0.9962888095608153</v>
       </c>
       <c r="AC5">
-        <v>0.9706964951149191</v>
+        <v>0.9935350843480851</v>
       </c>
       <c r="AD5">
-        <v>0.9606006129477037</v>
+        <v>0.9917844829845989</v>
       </c>
       <c r="AE5">
-        <v>0.9557951580406527</v>
+        <v>0.9910350484342844</v>
       </c>
       <c r="AF5">
-        <v>0.9517901133143443</v>
+        <v>0.9901136720427188</v>
       </c>
       <c r="AG5">
-        <v>0.9509090888220104</v>
+        <v>0.9900496103216828</v>
       </c>
       <c r="AH5">
-        <v>0.950636396003318</v>
+        <v>0.9900504348713953</v>
       </c>
     </row>
     <row r="6" spans="1:34">
@@ -897,100 +897,100 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.9987512875163196</v>
+        <v>0.999653442343536</v>
       </c>
       <c r="D6">
-        <v>0.9947571646904807</v>
+        <v>0.9986307164923518</v>
       </c>
       <c r="E6">
-        <v>0.9968653165045861</v>
+        <v>0.9992388572359437</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.9902211337167808</v>
+        <v>0.9977024707775228</v>
       </c>
       <c r="H6">
-        <v>0.9974238615992018</v>
+        <v>1.000017832747143</v>
       </c>
       <c r="I6">
-        <v>0.9871342674465871</v>
+        <v>0.9971176107117705</v>
       </c>
       <c r="J6">
-        <v>0.9924326280834291</v>
+        <v>0.9984354971967386</v>
       </c>
       <c r="K6">
-        <v>0.9992807908022433</v>
+        <v>0.9999886857992298</v>
       </c>
       <c r="L6">
-        <v>0.9994721684155937</v>
+        <v>0.9999646643204834</v>
       </c>
       <c r="M6">
-        <v>0.9999999999999998</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>0.9937149367136483</v>
+        <v>0.9975302014980475</v>
       </c>
       <c r="O6">
-        <v>0.9909139192966995</v>
+        <v>0.9968542290302802</v>
       </c>
       <c r="P6">
-        <v>0.9896114238343148</v>
+        <v>0.996236739519973</v>
       </c>
       <c r="Q6">
-        <v>0.9883486428311873</v>
+        <v>0.9956114665337311</v>
       </c>
       <c r="R6">
-        <v>0.9864792227021054</v>
+        <v>0.9948038298840988</v>
       </c>
       <c r="S6">
-        <v>0.9859178889485899</v>
+        <v>0.9945732703964146</v>
       </c>
       <c r="T6">
-        <v>0.9971095214076882</v>
+        <v>0.9994566664603406</v>
       </c>
       <c r="U6">
-        <v>0.9924658318011671</v>
+        <v>0.998009821474874</v>
       </c>
       <c r="V6">
-        <v>0.9914939657936234</v>
+        <v>0.9977538296012932</v>
       </c>
       <c r="W6">
-        <v>0.990392283428389</v>
+        <v>0.9975317830990375</v>
       </c>
       <c r="X6">
-        <v>0.9893722645972168</v>
+        <v>0.9972080391433421</v>
       </c>
       <c r="Y6">
-        <v>0.979118523612249</v>
+        <v>0.9956980348182088</v>
       </c>
       <c r="Z6">
-        <v>0.9722094165618103</v>
+        <v>0.9955104364459689</v>
       </c>
       <c r="AA6">
-        <v>0.9878168730830323</v>
+        <v>0.997088672931162</v>
       </c>
       <c r="AB6">
-        <v>0.9845816034630729</v>
+        <v>0.9962888095608164</v>
       </c>
       <c r="AC6">
-        <v>0.9706964951149148</v>
+        <v>0.9935350843480857</v>
       </c>
       <c r="AD6">
-        <v>0.9606006129476989</v>
+        <v>0.9917844829845995</v>
       </c>
       <c r="AE6">
-        <v>0.9557951580406476</v>
+        <v>0.9910350484342854</v>
       </c>
       <c r="AF6">
-        <v>0.9517901133143396</v>
+        <v>0.9901136720427205</v>
       </c>
       <c r="AG6">
-        <v>0.9509090888220058</v>
+        <v>0.9900496103216844</v>
       </c>
       <c r="AH6">
-        <v>0.9506363960033135</v>
+        <v>0.9900504348713968</v>
       </c>
     </row>
     <row r="7" spans="1:34">
@@ -1001,100 +1001,100 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.9987537966535432</v>
+        <v>0.9996434390555818</v>
       </c>
       <c r="D7">
-        <v>0.9947543440512199</v>
+        <v>0.9985908835064561</v>
       </c>
       <c r="E7">
-        <v>0.996878863548984</v>
+        <v>0.9992191891046173</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0.9900283554187503</v>
+        <v>0.9974276565729772</v>
       </c>
       <c r="H7">
-        <v>0.9967109352159922</v>
+        <v>0.9993061724635108</v>
       </c>
       <c r="I7">
-        <v>0.9873708748861865</v>
+        <v>0.9971470782422068</v>
       </c>
       <c r="J7">
-        <v>0.9925106447839964</v>
+        <v>0.998378553448624</v>
       </c>
       <c r="K7">
-        <v>0.9991635587073516</v>
+        <v>0.9998436226147908</v>
       </c>
       <c r="L7">
-        <v>0.9993970360977336</v>
+        <v>0.9998689529823007</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="N7">
-        <v>0.9945598367906706</v>
+        <v>0.9983459682778091</v>
       </c>
       <c r="O7">
-        <v>0.9920721144454033</v>
+        <v>0.9979790627517758</v>
       </c>
       <c r="P7">
-        <v>0.9907711656989568</v>
+        <v>0.9973399856357872</v>
       </c>
       <c r="Q7">
-        <v>0.9895098822299893</v>
+        <v>0.9966929082473986</v>
       </c>
       <c r="R7">
-        <v>0.9876426865222814</v>
+        <v>0.9958570139634573</v>
       </c>
       <c r="S7">
-        <v>0.9870820169069235</v>
+        <v>0.9956184402032147</v>
       </c>
       <c r="T7">
-        <v>0.9971078010161363</v>
+        <v>0.9994390639980565</v>
       </c>
       <c r="U7">
-        <v>0.9924276470187063</v>
+        <v>0.9979400020727318</v>
       </c>
       <c r="V7">
-        <v>0.9914461096336264</v>
+        <v>0.9976747614952796</v>
       </c>
       <c r="W7">
-        <v>0.9903277416100066</v>
+        <v>0.9974447103449525</v>
       </c>
       <c r="X7">
-        <v>0.9893025800628559</v>
+        <v>0.997117090361926</v>
       </c>
       <c r="Y7">
-        <v>0.978916069776595</v>
+        <v>0.9955527805054498</v>
       </c>
       <c r="Z7">
-        <v>0.9718760039092726</v>
+        <v>0.9953584126113203</v>
       </c>
       <c r="AA7">
-        <v>0.9876033101274592</v>
+        <v>0.9967914902674225</v>
       </c>
       <c r="AB7">
-        <v>0.9843389592745915</v>
+        <v>0.9959624748978025</v>
       </c>
       <c r="AC7">
-        <v>0.9703439113952175</v>
+        <v>0.9931080668548579</v>
       </c>
       <c r="AD7">
-        <v>0.9601648556057408</v>
+        <v>0.9912935388530264</v>
       </c>
       <c r="AE7">
-        <v>0.9553077064559472</v>
+        <v>0.9905167998032968</v>
       </c>
       <c r="AF7">
-        <v>0.9513005894554846</v>
+        <v>0.9895616915204151</v>
       </c>
       <c r="AG7">
-        <v>0.9504191089463575</v>
+        <v>0.9894952423681465</v>
       </c>
       <c r="AH7">
-        <v>0.9501462746380891</v>
+        <v>0.9894960664561606</v>
       </c>
     </row>
     <row r="8" spans="1:34">
@@ -1105,100 +1105,100 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.9987360020160713</v>
+        <v>0.999608728411036</v>
       </c>
       <c r="D8">
-        <v>0.9946490266444247</v>
+        <v>0.9984536167403096</v>
       </c>
       <c r="E8">
-        <v>0.9968398582926667</v>
+        <v>0.9991457125534955</v>
       </c>
       <c r="F8">
         <v>0.9999999999999999</v>
       </c>
       <c r="G8">
-        <v>0.989654018317731</v>
+        <v>0.9969121377489121</v>
       </c>
       <c r="H8">
-        <v>0.9957489625948467</v>
+        <v>0.9983470994269265</v>
       </c>
       <c r="I8">
-        <v>0.9875048637306558</v>
+        <v>0.996993767049386</v>
       </c>
       <c r="J8">
-        <v>0.992486148320857</v>
+        <v>0.9981933956529844</v>
       </c>
       <c r="K8">
-        <v>0.9989904863762683</v>
+        <v>0.9996442176362353</v>
       </c>
       <c r="L8">
-        <v>0.9992853736724746</v>
+        <v>0.9997356014626776</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="N8">
-        <v>0.9956181596607718</v>
+        <v>0.9993327677053639</v>
       </c>
       <c r="O8">
-        <v>0.9935226695162938</v>
+        <v>0.9993538930241318</v>
       </c>
       <c r="P8">
-        <v>0.9922236527910797</v>
+        <v>0.9986488797795217</v>
       </c>
       <c r="Q8">
-        <v>0.9909642398994194</v>
+        <v>0.9979352085528224</v>
       </c>
       <c r="R8">
-        <v>0.9890998227175452</v>
+        <v>0.9970130023774642</v>
       </c>
       <c r="S8">
-        <v>0.9885399826727079</v>
+        <v>0.9967499547314826</v>
       </c>
       <c r="T8">
-        <v>0.9970772446866755</v>
+        <v>0.9993815058016841</v>
       </c>
       <c r="U8">
-        <v>0.992287525580959</v>
+        <v>0.9977257169263483</v>
       </c>
       <c r="V8">
-        <v>0.9912769364286949</v>
+        <v>0.9974327181524626</v>
       </c>
       <c r="W8">
-        <v>0.9901084650587706</v>
+        <v>0.997178642743486</v>
       </c>
       <c r="X8">
-        <v>0.9889956885085327</v>
+        <v>0.9968263554586756</v>
       </c>
       <c r="Y8">
-        <v>0.9782090109379682</v>
+        <v>0.9950989904202406</v>
       </c>
       <c r="Z8">
-        <v>0.9707746887762827</v>
+        <v>0.9948842974432628</v>
       </c>
       <c r="AA8">
-        <v>0.9871670143712249</v>
+        <v>0.9962089368594146</v>
       </c>
       <c r="AB8">
-        <v>0.9838159477720642</v>
+        <v>0.9952925531783496</v>
       </c>
       <c r="AC8">
-        <v>0.9694934149192137</v>
+        <v>0.9921363586420828</v>
       </c>
       <c r="AD8">
-        <v>0.9590665814143668</v>
+        <v>0.9901302441769728</v>
       </c>
       <c r="AE8">
-        <v>0.9540551361240853</v>
+        <v>0.9892716785745868</v>
       </c>
       <c r="AF8">
-        <v>0.9500426842987394</v>
+        <v>0.9882154772426003</v>
       </c>
       <c r="AG8">
-        <v>0.9491600298275057</v>
+        <v>0.9881418738140022</v>
       </c>
       <c r="AH8">
-        <v>0.9488868312711897</v>
+        <v>0.9881426967748814</v>
       </c>
     </row>
     <row r="9" spans="1:34">
@@ -1209,100 +1209,100 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0.9986728356629014</v>
+        <v>0.9995328419562176</v>
       </c>
       <c r="D9">
-        <v>0.9943326448121371</v>
+        <v>0.9981547777975508</v>
       </c>
       <c r="E9">
-        <v>0.9966753210177363</v>
+        <v>0.9989791413752457</v>
       </c>
       <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0.9961012012399648</v>
+      </c>
+      <c r="H9">
+        <v>0.997249784594787</v>
+      </c>
+      <c r="I9">
+        <v>0.9965350704753821</v>
+      </c>
+      <c r="J9">
+        <v>0.9978256198419976</v>
+      </c>
+      <c r="K9">
+        <v>0.9994131093305711</v>
+      </c>
+      <c r="L9">
+        <v>0.9995784187946319</v>
+      </c>
+      <c r="M9">
         <v>0.9999999999999999</v>
       </c>
-      <c r="G9">
-        <v>0.9890549062791639</v>
-      </c>
-      <c r="H9">
-        <v>0.9946469632335594</v>
-      </c>
-      <c r="I9">
-        <v>0.9873950856495389</v>
-      </c>
-      <c r="J9">
-        <v>0.9922746147846806</v>
-      </c>
-      <c r="K9">
-        <v>0.9987734105092557</v>
-      </c>
-      <c r="L9">
-        <v>0.999144500868312</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
       <c r="N9">
-        <v>0.9967043893108101</v>
+        <v>1.000287037992768</v>
       </c>
       <c r="O9">
-        <v>0.9950112420244996</v>
+        <v>1.000707915989438</v>
       </c>
       <c r="P9">
-        <v>0.9937142020528259</v>
+        <v>0.9998702646264906</v>
       </c>
       <c r="Q9">
-        <v>0.9924567030362111</v>
+        <v>0.9990226395399325</v>
       </c>
       <c r="R9">
-        <v>0.9905951286826447</v>
+        <v>0.9979267977853392</v>
       </c>
       <c r="S9">
-        <v>0.9900361374012703</v>
+        <v>0.9976145278899238</v>
       </c>
       <c r="T9">
-        <v>0.996988372550202</v>
+        <v>0.9992597015724775</v>
       </c>
       <c r="U9">
-        <v>0.991979148940783</v>
+        <v>0.9972901338317303</v>
       </c>
       <c r="V9">
-        <v>0.9909103699350217</v>
+        <v>0.9969415674154996</v>
       </c>
       <c r="W9">
-        <v>0.9896415755229253</v>
+        <v>0.9966393997787857</v>
       </c>
       <c r="X9">
-        <v>0.9882735116920282</v>
+        <v>0.9962201031613598</v>
       </c>
       <c r="Y9">
-        <v>0.9766815067804928</v>
+        <v>0.9941660743198679</v>
       </c>
       <c r="Z9">
-        <v>0.9684546892455618</v>
+        <v>0.993910665651177</v>
       </c>
       <c r="AA9">
-        <v>0.9864437940229274</v>
+        <v>0.9952635603594772</v>
       </c>
       <c r="AB9">
-        <v>0.9829190168606357</v>
+        <v>0.9941719359526792</v>
       </c>
       <c r="AC9">
-        <v>0.967940560129206</v>
+        <v>0.9904102319781111</v>
       </c>
       <c r="AD9">
-        <v>0.9570176865080371</v>
+        <v>0.9880198396493789</v>
       </c>
       <c r="AE9">
-        <v>0.9516972400643487</v>
+        <v>0.9869971704732673</v>
       </c>
       <c r="AF9">
-        <v>0.9476747070893945</v>
+        <v>0.985738199624598</v>
       </c>
       <c r="AG9">
-        <v>0.9467898341941109</v>
+        <v>0.9856502484259259</v>
       </c>
       <c r="AH9">
-        <v>0.9465159473235174</v>
+        <v>0.9856510693116877</v>
       </c>
     </row>
     <row r="10" spans="1:34">
@@ -1313,100 +1313,100 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0.9986149645383039</v>
+        <v>0.9994628573201547</v>
       </c>
       <c r="D10">
-        <v>0.994042167918775</v>
+        <v>0.9978793179160572</v>
       </c>
       <c r="E10">
-        <v>0.996524661703862</v>
+        <v>0.9988254086104815</v>
       </c>
       <c r="F10">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G10">
-        <v>0.9885146939356902</v>
+        <v>0.9953762136427934</v>
       </c>
       <c r="H10">
-        <v>0.9937131265090702</v>
+        <v>0.9963203797588325</v>
       </c>
       <c r="I10">
-        <v>0.9872471846640686</v>
+        <v>0.9960970754696535</v>
       </c>
       <c r="J10">
-        <v>0.9920569877908731</v>
+        <v>0.9974866758388242</v>
       </c>
       <c r="K10">
-        <v>0.9985847248532663</v>
+        <v>0.9992167610619448</v>
       </c>
       <c r="L10">
-        <v>0.999021835129524</v>
+        <v>0.9994444423863987</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="N10">
-        <v>0.9976015471409269</v>
+        <v>1.001064451598215</v>
       </c>
       <c r="O10">
-        <v>0.9962405334877132</v>
+        <v>1.001815562318277</v>
       </c>
       <c r="P10">
-        <v>0.9949451214673993</v>
+        <v>1.000856369803731</v>
       </c>
       <c r="Q10">
-        <v>0.9936891986095997</v>
+        <v>0.9998860039383882</v>
       </c>
       <c r="R10">
-        <v>0.9918299654394749</v>
+        <v>0.9986310436277298</v>
       </c>
       <c r="S10">
-        <v>0.9912716731447277</v>
+        <v>0.9982736789433853</v>
       </c>
       <c r="T10">
-        <v>0.9969067794077232</v>
+        <v>0.9991473658293482</v>
       </c>
       <c r="U10">
-        <v>0.9916960590262069</v>
+        <v>0.9968897963314536</v>
       </c>
       <c r="V10">
-        <v>0.9905738705079294</v>
+        <v>0.9964902345764768</v>
       </c>
       <c r="W10">
-        <v>0.9892130136947306</v>
+        <v>0.9961439326645853</v>
       </c>
       <c r="X10">
-        <v>0.9876086357997601</v>
+        <v>0.9956623259832662</v>
       </c>
       <c r="Y10">
-        <v>0.9752738601065231</v>
+        <v>0.9933082460307731</v>
       </c>
       <c r="Z10">
-        <v>0.9663167924820213</v>
+        <v>0.9930154427880079</v>
       </c>
       <c r="AA10">
-        <v>0.9857891503547709</v>
+        <v>0.9944147458253003</v>
       </c>
       <c r="AB10">
-        <v>0.9821042156171815</v>
+        <v>0.9931616899540295</v>
       </c>
       <c r="AC10">
-        <v>0.966520812811914</v>
+        <v>0.9888419575959496</v>
       </c>
       <c r="AD10">
-        <v>0.9551408042745015</v>
+        <v>0.9860975674748278</v>
       </c>
       <c r="AE10">
-        <v>0.9495357376955943</v>
+        <v>0.9849237513860847</v>
       </c>
       <c r="AF10">
-        <v>0.9455039186471402</v>
+        <v>0.9834779874944305</v>
       </c>
       <c r="AG10">
-        <v>0.9446170022860705</v>
+        <v>0.9833768211844317</v>
       </c>
       <c r="AH10">
-        <v>0.9443424813875069</v>
+        <v>0.9833776401767998</v>
       </c>
     </row>
     <row r="11" spans="1:34">
@@ -1417,100 +1417,100 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.9985715349405575</v>
+        <v>0.9994112865420768</v>
       </c>
       <c r="D11">
-        <v>0.9938254560181826</v>
+        <v>0.9976764953325058</v>
       </c>
       <c r="E11">
-        <v>0.9964109498969538</v>
+        <v>0.9987117016484176</v>
       </c>
       <c r="F11">
-        <v>0.9999999999999998</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G11">
-        <v>0.9881330492298962</v>
+        <v>0.9948663383562243</v>
       </c>
       <c r="H11">
-        <v>0.9931013220131362</v>
+        <v>0.9957116834875621</v>
       </c>
       <c r="I11">
-        <v>0.9871075045710394</v>
+        <v>0.9957662948496045</v>
       </c>
       <c r="J11">
-        <v>0.9918847512911807</v>
+        <v>0.9972408277037553</v>
       </c>
       <c r="K11">
-        <v>0.998458111760508</v>
+        <v>0.9990880205773111</v>
       </c>
       <c r="L11">
-        <v>0.9989394010599909</v>
+        <v>0.9993561955134344</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="N11">
-        <v>0.9981683971486592</v>
+        <v>1.001545156516219</v>
       </c>
       <c r="O11">
-        <v>0.9970171530769131</v>
+        <v>1.002505073150781</v>
       </c>
       <c r="P11">
-        <v>0.9957227674485927</v>
+        <v>1.001457447557096</v>
       </c>
       <c r="Q11">
-        <v>0.9944678383243595</v>
+        <v>1.000397779430575</v>
       </c>
       <c r="R11">
-        <v>0.9926100812151052</v>
+        <v>0.9990270387420723</v>
       </c>
       <c r="S11">
-        <v>0.9920522296129519</v>
+        <v>0.9986368688461187</v>
       </c>
       <c r="T11">
-        <v>0.9968459995519118</v>
+        <v>0.9990648375415702</v>
       </c>
       <c r="U11">
-        <v>0.9914885572816412</v>
+        <v>0.9965975872674911</v>
       </c>
       <c r="V11">
-        <v>0.990327482389599</v>
+        <v>0.9961609026032709</v>
       </c>
       <c r="W11">
-        <v>0.9888996090794301</v>
+        <v>0.9957824728607533</v>
       </c>
       <c r="X11">
-        <v>0.9871181234749682</v>
+        <v>0.9952538624357984</v>
       </c>
       <c r="Y11">
-        <v>0.974240305775704</v>
+        <v>0.9926811909017743</v>
       </c>
       <c r="Z11">
-        <v>0.9647497821289046</v>
+        <v>0.9923611476329306</v>
       </c>
       <c r="AA11">
-        <v>0.9853238980857723</v>
+        <v>0.9938144672178919</v>
       </c>
       <c r="AB11">
-        <v>0.981521950822679</v>
+        <v>0.9924435387392492</v>
       </c>
       <c r="AC11">
-        <v>0.9654964593625527</v>
+        <v>0.9877162074712235</v>
       </c>
       <c r="AD11">
-        <v>0.9537825923000753</v>
+        <v>0.9847133364357552</v>
       </c>
       <c r="AE11">
-        <v>0.9479697385622424</v>
+        <v>0.9834291719720346</v>
       </c>
       <c r="AF11">
-        <v>0.9439311649669528</v>
+        <v>0.9818470153056713</v>
       </c>
       <c r="AG11">
-        <v>0.9430427622182149</v>
+        <v>0.9817362009025317</v>
       </c>
       <c r="AH11">
-        <v>0.9427677801378213</v>
+        <v>0.9817370185285311</v>
       </c>
     </row>
     <row r="12" spans="1:34">
@@ -1521,100 +1521,100 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>0.9985512676367346</v>
+        <v>0.9993861328333592</v>
       </c>
       <c r="D12">
-        <v>0.9937224893379142</v>
+        <v>0.9975774551059431</v>
       </c>
       <c r="E12">
-        <v>0.9963586142044463</v>
+        <v>0.9986568056694551</v>
       </c>
       <c r="F12">
         <v>0.9999999999999998</v>
       </c>
       <c r="G12">
-        <v>0.9879713459267458</v>
+        <v>0.9946490299896991</v>
       </c>
       <c r="H12">
-        <v>0.9929308037632463</v>
+        <v>0.9955421168550831</v>
       </c>
       <c r="I12">
-        <v>0.9869900352119855</v>
+        <v>0.9955815200815974</v>
       </c>
       <c r="J12">
-        <v>0.9917826396410099</v>
+        <v>0.9971225716073367</v>
       </c>
       <c r="K12">
-        <v>0.9984185807552416</v>
+        <v>0.9990522201964243</v>
       </c>
       <c r="L12">
-        <v>0.9989135278928885</v>
+        <v>0.9993307783530332</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
       <c r="N12">
-        <v>0.9982831989036756</v>
+        <v>1.001618518933114</v>
       </c>
       <c r="O12">
-        <v>0.9971744308760058</v>
+        <v>1.002621331152805</v>
       </c>
       <c r="P12">
-        <v>0.995880252912139</v>
+        <v>1.001529253880501</v>
       </c>
       <c r="Q12">
-        <v>0.9946255248443547</v>
+        <v>1.000424698680082</v>
       </c>
       <c r="R12">
-        <v>0.9927680663777144</v>
+        <v>0.9989957578261125</v>
       </c>
       <c r="S12">
-        <v>0.9922103039380864</v>
+        <v>0.9985891002052979</v>
       </c>
       <c r="T12">
-        <v>0.9968170295475183</v>
+        <v>0.9990241558176548</v>
       </c>
       <c r="U12">
-        <v>0.9913861800042942</v>
+        <v>0.9964519960299595</v>
       </c>
       <c r="V12">
-        <v>0.9902056505057202</v>
+        <v>0.9959967390754723</v>
       </c>
       <c r="W12">
-        <v>0.9887442520339338</v>
+        <v>0.9956022361825696</v>
       </c>
       <c r="X12">
-        <v>0.9868778259238208</v>
+        <v>0.9950519082225842</v>
       </c>
       <c r="Y12">
-        <v>0.9737276773136007</v>
+        <v>0.9923698309582212</v>
       </c>
       <c r="Z12">
-        <v>0.9639697429239941</v>
+        <v>0.9920361547574577</v>
       </c>
       <c r="AA12">
-        <v>0.9851203494668289</v>
+        <v>0.9935518847648539</v>
       </c>
       <c r="AB12">
-        <v>0.9812598357495254</v>
+        <v>0.9921219207796221</v>
       </c>
       <c r="AC12">
-        <v>0.9650130864943404</v>
+        <v>0.987190402022843</v>
       </c>
       <c r="AD12">
-        <v>0.9531321849463661</v>
+        <v>0.9840580722701111</v>
       </c>
       <c r="AE12">
-        <v>0.9472153554798944</v>
+        <v>0.9827186453014489</v>
       </c>
       <c r="AF12">
-        <v>0.9431735199576994</v>
+        <v>0.9810681768493249</v>
       </c>
       <c r="AG12">
-        <v>0.9422843993973308</v>
+        <v>0.9809525306956565</v>
       </c>
       <c r="AH12">
-        <v>0.9420091946016661</v>
+        <v>0.9809533476689865</v>
       </c>
     </row>
     <row r="13" spans="1:34">
@@ -1625,100 +1625,100 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>0.9985435315917389</v>
+        <v>0.9993790462312945</v>
       </c>
       <c r="D13">
-        <v>0.9936865931449214</v>
+        <v>0.9975497118670756</v>
       </c>
       <c r="E13">
-        <v>0.9963372259381883</v>
+        <v>0.998640668888186</v>
       </c>
       <c r="F13">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0.9879573282873265</v>
+        <v>0.9946283034236306</v>
       </c>
       <c r="H13">
-        <v>0.993008476500123</v>
+        <v>0.9956194621851779</v>
       </c>
       <c r="I13">
-        <v>0.9869194922645502</v>
+        <v>0.995518106625031</v>
       </c>
       <c r="J13">
-        <v>0.9917436935286411</v>
+        <v>0.9970970902377281</v>
       </c>
       <c r="K13">
-        <v>0.9984299601233455</v>
+        <v>0.9990685809266199</v>
       </c>
       <c r="L13">
-        <v>0.9989207902173313</v>
+        <v>0.9993409948945713</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>0.9981624562790636</v>
+        <v>1.001488837951281</v>
       </c>
       <c r="O13">
-        <v>0.9970090140462815</v>
+        <v>1.002447893276329</v>
       </c>
       <c r="P13">
-        <v>0.9957146176696544</v>
+        <v>1.001344474344574</v>
       </c>
       <c r="Q13">
-        <v>0.9944596781391285</v>
+        <v>1.000228466878152</v>
       </c>
       <c r="R13">
-        <v>0.9926019055727071</v>
+        <v>0.9987846760994388</v>
       </c>
       <c r="S13">
-        <v>0.9920440493556715</v>
+        <v>0.9983738122203778</v>
       </c>
       <c r="T13">
-        <v>0.996807109788296</v>
+        <v>0.9990131817228606</v>
       </c>
       <c r="U13">
-        <v>0.991357887850471</v>
+        <v>0.9964147850820123</v>
       </c>
       <c r="V13">
-        <v>0.9901724900852662</v>
+        <v>0.9959548835236743</v>
       </c>
       <c r="W13">
-        <v>0.9887027043264645</v>
+        <v>0.9955563610332385</v>
       </c>
       <c r="X13">
-        <v>0.9868074729499234</v>
+        <v>0.9949984184470296</v>
       </c>
       <c r="Y13">
-        <v>0.9735890050317187</v>
+        <v>0.9922889694606364</v>
       </c>
       <c r="Z13">
-        <v>0.9637640337796448</v>
+        <v>0.9919518825784666</v>
       </c>
       <c r="AA13">
-        <v>0.9850959401723061</v>
+        <v>0.9935198668809535</v>
       </c>
       <c r="AB13">
-        <v>0.9812208790313725</v>
+        <v>0.9920751790168455</v>
       </c>
       <c r="AC13">
-        <v>0.9649192175415007</v>
+        <v>0.9870927301918297</v>
       </c>
       <c r="AD13">
-        <v>0.9529968569020399</v>
+        <v>0.9839281125202274</v>
       </c>
       <c r="AE13">
-        <v>0.9470541799423163</v>
+        <v>0.9825749031264638</v>
       </c>
       <c r="AF13">
-        <v>0.943011646819276</v>
+        <v>0.9809073972768633</v>
       </c>
       <c r="AG13">
-        <v>0.9421223727465228</v>
+        <v>0.9807905461334764</v>
       </c>
       <c r="AH13">
-        <v>0.9418471203206269</v>
+        <v>0.9807913629718997</v>
       </c>
     </row>
     <row r="14" spans="1:34">
@@ -1729,100 +1729,100 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0.998512659302358</v>
+        <v>0.9993727167657627</v>
       </c>
       <c r="D14">
-        <v>0.9935757121845001</v>
+        <v>0.9975272088248975</v>
       </c>
       <c r="E14">
-        <v>0.9962383741883289</v>
+        <v>0.9986160355107946</v>
       </c>
       <c r="F14">
-        <v>0.9999999999999998</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0.9881198403545159</v>
+        <v>0.9948398863489596</v>
       </c>
       <c r="H14">
-        <v>0.9936193363489569</v>
+        <v>0.9962275893419125</v>
       </c>
       <c r="I14">
-        <v>0.9867456631427054</v>
+        <v>0.9954776706815949</v>
       </c>
       <c r="J14">
-        <v>0.9916994303876021</v>
+        <v>0.9971420044177126</v>
       </c>
       <c r="K14">
-        <v>0.9985387763026465</v>
+        <v>0.9991961776814683</v>
       </c>
       <c r="L14">
-        <v>0.9989910665787447</v>
+        <v>0.999424984737481</v>
       </c>
       <c r="M14">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>0.9974273021409137</v>
+        <v>1.000770810815022</v>
       </c>
       <c r="O14">
-        <v>0.9960017943159428</v>
+        <v>1.00146156584693</v>
       </c>
       <c r="P14">
-        <v>0.9947060664501652</v>
+        <v>1.000368197452827</v>
       </c>
       <c r="Q14">
-        <v>0.9934498377960266</v>
+        <v>0.9992623405791429</v>
       </c>
       <c r="R14">
-        <v>0.9915901504049357</v>
+        <v>0.9978317081783533</v>
       </c>
       <c r="S14">
-        <v>0.9910317224977137</v>
+        <v>0.99742457355044</v>
       </c>
       <c r="T14">
-        <v>0.9967783505495644</v>
+        <v>0.9990107342866898</v>
       </c>
       <c r="U14">
-        <v>0.9913472856837658</v>
+        <v>0.9964385393434155</v>
       </c>
       <c r="V14">
-        <v>0.9901667093709541</v>
+        <v>0.9959832761643008</v>
       </c>
       <c r="W14">
-        <v>0.9887052530576058</v>
+        <v>0.995588767891198</v>
       </c>
       <c r="X14">
-        <v>0.9867299692961202</v>
+        <v>0.9950015331049826</v>
       </c>
       <c r="Y14">
-        <v>0.9735777464333568</v>
+        <v>0.992319318729062</v>
       </c>
       <c r="Z14">
-        <v>0.9638182729009266</v>
+        <v>0.9919856254168252</v>
       </c>
       <c r="AA14">
-        <v>0.9852693093378384</v>
+        <v>0.9937429585770684</v>
       </c>
       <c r="AB14">
-        <v>0.981409427295052</v>
+        <v>0.992313278282941</v>
       </c>
       <c r="AC14">
-        <v>0.9651653494366449</v>
+        <v>0.9873827435974093</v>
       </c>
       <c r="AD14">
-        <v>0.9532864014259188</v>
+        <v>0.9842510366042742</v>
       </c>
       <c r="AE14">
-        <v>0.947370544999406</v>
+        <v>0.9829118750198103</v>
       </c>
       <c r="AF14">
-        <v>0.9433293809418587</v>
+        <v>0.9812617356326618</v>
       </c>
       <c r="AG14">
-        <v>0.9424404081423876</v>
+        <v>0.9811461129601994</v>
       </c>
       <c r="AH14">
-        <v>0.9421652491924508</v>
+        <v>0.9811469300947516</v>
       </c>
     </row>
     <row r="15" spans="1:34">
@@ -1833,100 +1833,100 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0.9984761018583309</v>
+        <v>0.999356091477611</v>
       </c>
       <c r="D15">
-        <v>0.9934301779711638</v>
+        <v>0.9974636513938611</v>
       </c>
       <c r="E15">
-        <v>0.9961271339461186</v>
+        <v>0.9985707695079835</v>
       </c>
       <c r="F15">
         <v>0.9999999999999997</v>
       </c>
       <c r="G15">
-        <v>0.9882993472763797</v>
+        <v>0.9950772349542439</v>
       </c>
       <c r="H15">
-        <v>0.9946654933005435</v>
+        <v>0.9972697693003159</v>
       </c>
       <c r="I15">
-        <v>0.9862841713528017</v>
+        <v>0.9952356792271079</v>
       </c>
       <c r="J15">
-        <v>0.9915091057378685</v>
+        <v>0.9971202558938937</v>
       </c>
       <c r="K15">
-        <v>0.9987115084231626</v>
+        <v>0.9994098799380744</v>
       </c>
       <c r="L15">
-        <v>0.9991019893531792</v>
+        <v>0.999564100102641</v>
       </c>
       <c r="M15">
-        <v>0.9999999999999999</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="N15">
-        <v>0.9960981399616489</v>
+        <v>0.9994443146207819</v>
       </c>
       <c r="O15">
-        <v>0.9941804649403656</v>
+        <v>0.9996504698220164</v>
       </c>
       <c r="P15">
-        <v>0.9928823224720495</v>
+        <v>0.9985438985396737</v>
       </c>
       <c r="Q15">
-        <v>0.9916237560295668</v>
+        <v>0.9974247129305418</v>
       </c>
       <c r="R15">
-        <v>0.9897605961462717</v>
+        <v>0.995976792116313</v>
       </c>
       <c r="S15">
-        <v>0.9892011314850117</v>
+        <v>0.9955647635907653</v>
       </c>
       <c r="T15">
-        <v>0.996739556451249</v>
+        <v>0.9989902175227598</v>
       </c>
       <c r="U15">
-        <v>0.9912899571327506</v>
+        <v>0.9963917601154862</v>
       </c>
       <c r="V15">
-        <v>0.9901044772594407</v>
+        <v>0.9959318477981658</v>
       </c>
       <c r="W15">
-        <v>0.988634589889006</v>
+        <v>0.9955333160082104</v>
       </c>
       <c r="X15">
-        <v>0.9865491612824543</v>
+        <v>0.9949121350218219</v>
       </c>
       <c r="Y15">
-        <v>0.9733270486511352</v>
+        <v>0.9922024487584846</v>
       </c>
       <c r="Z15">
-        <v>0.9634993685640606</v>
+        <v>0.9918653322652686</v>
       </c>
       <c r="AA15">
-        <v>0.9854390352154975</v>
+        <v>0.9939693151665686</v>
       </c>
       <c r="AB15">
-        <v>0.9815654346187324</v>
+        <v>0.9925253014797819</v>
       </c>
       <c r="AC15">
-        <v>0.9652699476682797</v>
+        <v>0.9875451913458337</v>
       </c>
       <c r="AD15">
-        <v>0.9533521027247592</v>
+        <v>0.9843820536181273</v>
       </c>
       <c r="AE15">
-        <v>0.9474116769281734</v>
+        <v>0.9830294748841533</v>
       </c>
       <c r="AF15">
-        <v>0.9433706908003729</v>
+        <v>0.9813627510243011</v>
       </c>
       <c r="AG15">
-        <v>0.9424817571556909</v>
+        <v>0.9812459556750955</v>
       </c>
       <c r="AH15">
-        <v>0.9422066103543004</v>
+        <v>0.9812467728928003</v>
       </c>
     </row>
     <row r="16" spans="1:34">
@@ -1937,100 +1937,100 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>0.9984378438042636</v>
+        <v>0.9993435353912717</v>
       </c>
       <c r="D16">
-        <v>0.9932845463648426</v>
+        <v>0.9974164288547901</v>
       </c>
       <c r="E16">
-        <v>0.9960077218235445</v>
+        <v>0.9985323040907383</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G16">
-        <v>0.9885221942730172</v>
+        <v>0.9953893096319865</v>
       </c>
       <c r="H16">
-        <v>0.9958860282272562</v>
+        <v>0.9984867614550303</v>
       </c>
       <c r="I16">
-        <v>0.9857264771051426</v>
+        <v>0.9949688243178774</v>
       </c>
       <c r="J16">
-        <v>0.9912710069054845</v>
+        <v>0.9970945744833856</v>
       </c>
       <c r="K16">
-        <v>0.9989041794896021</v>
+        <v>0.9996519585431333</v>
       </c>
       <c r="L16">
-        <v>0.9992251468710173</v>
+        <v>0.999721896835298</v>
       </c>
       <c r="M16">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="N16">
-        <v>0.9945692544389171</v>
+        <v>0.9979302434898778</v>
       </c>
       <c r="O16">
-        <v>0.9920850234193288</v>
+        <v>0.9975783205724599</v>
       </c>
       <c r="P16">
-        <v>0.9907840918917024</v>
+        <v>0.9964694027174731</v>
       </c>
       <c r="Q16">
-        <v>0.9895228250939976</v>
+        <v>0.9953478513274687</v>
       </c>
       <c r="R16">
-        <v>0.9876556541495668</v>
+        <v>0.9938968561562322</v>
       </c>
       <c r="S16">
-        <v>0.98709499192768</v>
+        <v>0.9934839606801534</v>
       </c>
       <c r="T16">
-        <v>0.9967012282595682</v>
+        <v>0.9989776562691064</v>
       </c>
       <c r="U16">
-        <v>0.9912514148007397</v>
+        <v>0.9963791656218381</v>
       </c>
       <c r="V16">
-        <v>0.9900658883361269</v>
+        <v>0.9959192474192202</v>
       </c>
       <c r="W16">
-        <v>0.9885959433073306</v>
+        <v>0.9955207105423113</v>
       </c>
       <c r="X16">
-        <v>0.986402452077448</v>
+        <v>0.9948647901293944</v>
       </c>
       <c r="Y16">
-        <v>0.9731782684982759</v>
+        <v>0.9921549736513049</v>
       </c>
       <c r="Z16">
-        <v>0.9633490492344329</v>
+        <v>0.9918178409079077</v>
       </c>
       <c r="AA16">
-        <v>0.9856625828762889</v>
+        <v>0.9942817487804749</v>
       </c>
       <c r="AB16">
-        <v>0.9817899332992244</v>
+        <v>0.9928382033740676</v>
       </c>
       <c r="AC16">
-        <v>0.9654984668267612</v>
+        <v>0.9878597176786316</v>
       </c>
       <c r="AD16">
-        <v>0.9535835622238757</v>
+        <v>0.9846976079136129</v>
       </c>
       <c r="AE16">
-        <v>0.9476446022434426</v>
+        <v>0.9833454672336027</v>
       </c>
       <c r="AF16">
-        <v>0.9436046234155335</v>
+        <v>0.9816792865410029</v>
       </c>
       <c r="AG16">
-        <v>0.9427159114348048</v>
+        <v>0.9815625299465863</v>
       </c>
       <c r="AH16">
-        <v>0.9424408334090396</v>
+        <v>0.9815633474279457</v>
       </c>
     </row>
     <row r="17" spans="1:34">
@@ -2041,100 +2041,100 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0.9984222322440209</v>
+        <v>0.9993532619131532</v>
       </c>
       <c r="D17">
-        <v>0.993244292878755</v>
+        <v>0.9974562024906607</v>
       </c>
       <c r="E17">
-        <v>0.9959504598192109</v>
+        <v>0.9985452703843192</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
-        <v>0.9888003795230459</v>
+        <v>0.9957909757168176</v>
       </c>
       <c r="H17">
-        <v>0.9969844860468738</v>
+        <v>0.9995831739300399</v>
       </c>
       <c r="I17">
-        <v>0.9853072464830528</v>
+        <v>0.9948627254323408</v>
       </c>
       <c r="J17">
-        <v>0.991111508244365</v>
+        <v>0.9971390313765693</v>
       </c>
       <c r="K17">
-        <v>0.9990763482845431</v>
+        <v>0.9998661193892846</v>
       </c>
       <c r="L17">
-        <v>0.999334992846009</v>
+        <v>0.9998627889013116</v>
       </c>
       <c r="M17">
         <v>1</v>
       </c>
       <c r="N17">
-        <v>0.9932620180805434</v>
+        <v>0.9966663406333832</v>
       </c>
       <c r="O17">
-        <v>0.9902929961076274</v>
+        <v>0.9958362052118571</v>
       </c>
       <c r="P17">
-        <v>0.9889896699291814</v>
+        <v>0.9947589763475141</v>
       </c>
       <c r="Q17">
-        <v>0.9877260846216811</v>
+        <v>0.9936694269603412</v>
       </c>
       <c r="R17">
-        <v>0.9858554697844909</v>
+        <v>0.9922599209667443</v>
       </c>
       <c r="S17">
-        <v>0.9852937793295142</v>
+        <v>0.9918587814770989</v>
       </c>
       <c r="T17">
-        <v>0.9966920940392687</v>
+        <v>0.9989990349136066</v>
       </c>
       <c r="U17">
-        <v>0.9912971817861899</v>
+        <v>0.9964792191085532</v>
       </c>
       <c r="V17">
-        <v>0.9901262133352793</v>
+        <v>0.996033228567452</v>
       </c>
       <c r="W17">
-        <v>0.9886813729276694</v>
+        <v>0.9956467451842576</v>
       </c>
       <c r="X17">
-        <v>0.9864644797790593</v>
+        <v>0.9949816919380345</v>
       </c>
       <c r="Y17">
-        <v>0.9734431664183348</v>
+        <v>0.9923538707483935</v>
       </c>
       <c r="Z17">
-        <v>0.963813523032335</v>
+        <v>0.9920269551834139</v>
       </c>
       <c r="AA17">
-        <v>0.9859726410900662</v>
+        <v>0.9947176279950057</v>
       </c>
       <c r="AB17">
-        <v>0.9821445795363689</v>
+        <v>0.9933186960363261</v>
       </c>
       <c r="AC17">
-        <v>0.9660218671411276</v>
+        <v>0.9884945269735901</v>
       </c>
       <c r="AD17">
-        <v>0.9542342818128199</v>
+        <v>0.9854302508288093</v>
       </c>
       <c r="AE17">
-        <v>0.9483743148569126</v>
+        <v>0.9841198713556715</v>
       </c>
       <c r="AF17">
-        <v>0.9443374884678055</v>
+        <v>0.98250531537979</v>
       </c>
       <c r="AG17">
-        <v>0.9434494702048003</v>
+        <v>0.9823922104347679</v>
       </c>
       <c r="AH17">
-        <v>0.9431746074187987</v>
+        <v>0.9823930286071157</v>
       </c>
     </row>
     <row r="18" spans="1:34">
@@ -2145,100 +2145,100 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>0.9984244551396202</v>
+        <v>0.9993584799776012</v>
       </c>
       <c r="D18">
-        <v>0.9932591446837653</v>
+        <v>0.9974768966722936</v>
       </c>
       <c r="E18">
-        <v>0.9959545651003117</v>
+        <v>0.9985556563846918</v>
       </c>
       <c r="F18">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>0.9888339372138165</v>
+        <v>0.9958357891733026</v>
       </c>
       <c r="H18">
-        <v>0.9969834454035447</v>
+        <v>0.9995821005216294</v>
       </c>
       <c r="I18">
-        <v>0.9853596563964543</v>
+        <v>0.9949230084485097</v>
       </c>
       <c r="J18">
-        <v>0.9911477198543058</v>
+        <v>0.9971727497206911</v>
       </c>
       <c r="K18">
-        <v>0.9990797848997445</v>
+        <v>0.9998671165945338</v>
       </c>
       <c r="L18">
-        <v>0.9993373682411453</v>
+        <v>0.9998639928133989</v>
       </c>
       <c r="M18">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="N18">
-        <v>0.9932883812096694</v>
+        <v>0.9967026257293642</v>
       </c>
       <c r="O18">
-        <v>0.9903291394447112</v>
+        <v>0.9958818766434666</v>
       </c>
       <c r="P18">
-        <v>0.9890258616502295</v>
+        <v>0.9948159184899122</v>
       </c>
       <c r="Q18">
-        <v>0.9877623231884379</v>
+        <v>0.9937377500358926</v>
       </c>
       <c r="R18">
-        <v>0.9858917779355926</v>
+        <v>0.9923430008130185</v>
       </c>
       <c r="S18">
-        <v>0.9853301082562931</v>
+        <v>0.9919460416012267</v>
       </c>
       <c r="T18">
-        <v>0.9966964871772594</v>
+        <v>0.9990081337218483</v>
       </c>
       <c r="U18">
-        <v>0.9913199126055637</v>
+        <v>0.9965145423200933</v>
       </c>
       <c r="V18">
-        <v>0.9901538048364956</v>
+        <v>0.9960731943534644</v>
       </c>
       <c r="W18">
-        <v>0.9887173423482853</v>
+        <v>0.9956907288302629</v>
       </c>
       <c r="X18">
-        <v>0.9865135970734683</v>
+        <v>0.9950281069562206</v>
       </c>
       <c r="Y18">
-        <v>0.9735602387795723</v>
+        <v>0.9924276288388689</v>
       </c>
       <c r="Z18">
-        <v>0.9639973612393821</v>
+        <v>0.9921041204781107</v>
       </c>
       <c r="AA18">
-        <v>0.9860166267653302</v>
+        <v>0.9947737347344201</v>
       </c>
       <c r="AB18">
-        <v>0.9822031611081564</v>
+        <v>0.9933895285966613</v>
       </c>
       <c r="AC18">
-        <v>0.9661355752933971</v>
+        <v>0.9886162906179583</v>
       </c>
       <c r="AD18">
-        <v>0.9543896114446759</v>
+        <v>0.9855843066045953</v>
       </c>
       <c r="AE18">
-        <v>0.9485555654238339</v>
+        <v>0.9842877119540566</v>
       </c>
       <c r="AF18">
-        <v>0.9445195212945221</v>
+        <v>0.9826901956110569</v>
       </c>
       <c r="AG18">
-        <v>0.9436316751735709</v>
+        <v>0.9825782958955701</v>
       </c>
       <c r="AH18">
-        <v>0.9433568657981046</v>
+        <v>0.9825791142228967</v>
       </c>
     </row>
     <row r="19" spans="1:34">
@@ -2249,100 +2249,100 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>0.9983876810806391</v>
+        <v>0.999345779517825</v>
       </c>
       <c r="D19">
-        <v>0.993118970047863</v>
+        <v>0.9974289805943586</v>
       </c>
       <c r="E19">
-        <v>0.9958395029030201</v>
+        <v>0.9985165167106983</v>
       </c>
       <c r="F19">
         <v>0.9999999999999999</v>
       </c>
       <c r="G19">
-        <v>0.988944343038241</v>
+        <v>0.9960137635492335</v>
       </c>
       <c r="H19">
-        <v>0.9977444517935872</v>
+        <v>1.000342522147713</v>
       </c>
       <c r="I19">
-        <v>0.9849235620574922</v>
+        <v>0.9947033224952936</v>
       </c>
       <c r="J19">
-        <v>0.9909348947681288</v>
+        <v>0.9971179805142494</v>
       </c>
       <c r="K19">
-        <v>0.9991853527298467</v>
+        <v>1.000009624952903</v>
       </c>
       <c r="L19">
-        <v>0.9994039489734891</v>
+        <v>0.9999564582366884</v>
       </c>
       <c r="M19">
-        <v>0.9999999999999998</v>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>0.992327362646085</v>
+        <v>0.9957511366841415</v>
       </c>
       <c r="O19">
-        <v>0.9890115110948681</v>
+        <v>0.9945791964731643</v>
       </c>
       <c r="P19">
-        <v>0.9877064671279003</v>
+        <v>0.9935118129694422</v>
       </c>
       <c r="Q19">
-        <v>0.9864412186402945</v>
+        <v>0.9924322075369012</v>
       </c>
       <c r="R19">
-        <v>0.9845681333204825</v>
+        <v>0.9910355909240932</v>
       </c>
       <c r="S19">
-        <v>0.984005705255673</v>
+        <v>0.9906381051184675</v>
       </c>
       <c r="T19">
-        <v>0.9966596460934543</v>
+        <v>0.9989954282527266</v>
       </c>
       <c r="U19">
-        <v>0.9912828685035449</v>
+        <v>0.99650180458756</v>
       </c>
       <c r="V19">
-        <v>0.9901167166936878</v>
+        <v>0.9960604509079267</v>
       </c>
       <c r="W19">
-        <v>0.9886802000566072</v>
+        <v>0.9956779804468947</v>
       </c>
       <c r="X19">
-        <v>0.9863724073366993</v>
+        <v>0.9949800717707835</v>
       </c>
       <c r="Y19">
-        <v>0.9734170993474658</v>
+        <v>0.9923794669037111</v>
       </c>
       <c r="Z19">
-        <v>0.963852782259537</v>
+        <v>0.9920559427229655</v>
       </c>
       <c r="AA19">
-        <v>0.986127373904559</v>
+        <v>0.9949519050149152</v>
       </c>
       <c r="AB19">
-        <v>0.9823143712824324</v>
+        <v>0.993567954438438</v>
       </c>
       <c r="AC19">
-        <v>0.9662487457781928</v>
+        <v>0.9887956028351167</v>
       </c>
       <c r="AD19">
-        <v>0.9545042150866209</v>
+        <v>0.9857641798471077</v>
       </c>
       <c r="AE19">
-        <v>0.9486708810379691</v>
+        <v>0.98446782428146</v>
       </c>
       <c r="AF19">
-        <v>0.9446353344418371</v>
+        <v>0.9828706043960145</v>
       </c>
       <c r="AG19">
-        <v>0.9437475978067306</v>
+        <v>0.9827587258434274</v>
       </c>
       <c r="AH19">
-        <v>0.9434728224014556</v>
+        <v>0.982759544321023</v>
       </c>
     </row>
     <row r="20" spans="1:34">
@@ -2353,100 +2353,100 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0.9984100565279789</v>
+        <v>0.9993680072663254</v>
       </c>
       <c r="D20">
-        <v>0.9932233334488788</v>
+        <v>0.9975158421682347</v>
       </c>
       <c r="E20">
-        <v>0.9959009083406315</v>
+        <v>0.9985679083429964</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>0.9890439453692184</v>
+        <v>0.9961451170859743</v>
       </c>
       <c r="H20">
-        <v>0.9977217345019737</v>
+        <v>1.000319677285257</v>
       </c>
       <c r="I20">
-        <v>0.9850975193569017</v>
+        <v>0.9948944800724111</v>
       </c>
       <c r="J20">
-        <v>0.9910529912677352</v>
+        <v>0.9972239211484178</v>
       </c>
       <c r="K20">
-        <v>0.9991938402498098</v>
+        <v>1.000009702351177</v>
       </c>
       <c r="L20">
-        <v>0.9994099883293045</v>
+        <v>0.999958218209902</v>
       </c>
       <c r="M20">
-        <v>0.9999999999999994</v>
+        <v>1</v>
       </c>
       <c r="N20">
-        <v>0.9924316250688086</v>
+        <v>0.9958849483268964</v>
       </c>
       <c r="O20">
-        <v>0.989154471698359</v>
+        <v>0.9947503802341654</v>
       </c>
       <c r="P20">
-        <v>0.987849619587768</v>
+        <v>0.9937168770743728</v>
       </c>
       <c r="Q20">
-        <v>0.9865845568578852</v>
+        <v>0.9926714835156353</v>
       </c>
       <c r="R20">
-        <v>0.9847117474624592</v>
+        <v>0.9913192261059904</v>
       </c>
       <c r="S20">
-        <v>0.9841494017803579</v>
+        <v>0.9909343067867382</v>
       </c>
       <c r="T20">
-        <v>0.9966885536100518</v>
+        <v>0.9990292885801122</v>
       </c>
       <c r="U20">
-        <v>0.9913668641280045</v>
+        <v>0.9966143380029293</v>
       </c>
       <c r="V20">
-        <v>0.9902153103949649</v>
+        <v>0.9961869123760353</v>
       </c>
       <c r="W20">
-        <v>0.9888039467534796</v>
+        <v>0.9958164958123519</v>
       </c>
       <c r="X20">
-        <v>0.9865798979292734</v>
+        <v>0.9951441358310905</v>
       </c>
       <c r="Y20">
-        <v>0.9738290954651085</v>
+        <v>0.9926256001149657</v>
       </c>
       <c r="Z20">
-        <v>0.9644655340714297</v>
+        <v>0.9923123027307429</v>
       </c>
       <c r="AA20">
-        <v>0.9862582217224457</v>
+        <v>0.9951171026481768</v>
       </c>
       <c r="AB20">
-        <v>0.9824889535467832</v>
+        <v>0.9937772817051036</v>
       </c>
       <c r="AC20">
-        <v>0.9665884938612227</v>
+        <v>0.9891575464111485</v>
       </c>
       <c r="AD20">
-        <v>0.9549686837063339</v>
+        <v>0.9862228946979794</v>
       </c>
       <c r="AE20">
-        <v>0.9492130324844057</v>
+        <v>0.9849678499795546</v>
       </c>
       <c r="AF20">
-        <v>0.9451798233763068</v>
+        <v>0.9834216934353112</v>
       </c>
       <c r="AG20">
-        <v>0.9442926011225443</v>
+        <v>0.9833134267436641</v>
       </c>
       <c r="AH20">
-        <v>0.9440179853145176</v>
+        <v>0.9833142456832349</v>
       </c>
     </row>
     <row r="21" spans="1:34">
@@ -2457,100 +2457,100 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>0.9984178868184067</v>
+        <v>0.9993755498770094</v>
       </c>
       <c r="D21">
-        <v>0.9932595315092625</v>
+        <v>0.9975453015037495</v>
       </c>
       <c r="E21">
-        <v>0.9959225457094328</v>
+        <v>0.9985854560217751</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G21">
-        <v>0.989077001450867</v>
+        <v>0.99618872411756</v>
       </c>
       <c r="H21">
-        <v>0.9977141127015305</v>
+        <v>1.000312005980473</v>
       </c>
       <c r="I21">
-        <v>0.9851551955053179</v>
+        <v>0.994957815493862</v>
       </c>
       <c r="J21">
-        <v>0.9910921376126166</v>
+        <v>0.9972589632884235</v>
       </c>
       <c r="K21">
-        <v>0.9991966188234881</v>
+        <v>1.000009665299512</v>
       </c>
       <c r="L21">
-        <v>0.9994119663230439</v>
+        <v>0.9999587612068072</v>
       </c>
       <c r="M21">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="N21">
-        <v>0.9924663721806063</v>
+        <v>0.995929538368853</v>
       </c>
       <c r="O21">
-        <v>0.9892021151063737</v>
+        <v>0.9948074213152717</v>
       </c>
       <c r="P21">
-        <v>0.9878973269218972</v>
+        <v>0.993785206584672</v>
       </c>
       <c r="Q21">
-        <v>0.9866323260860449</v>
+        <v>0.9927512120136313</v>
       </c>
       <c r="R21">
-        <v>0.9847596086279431</v>
+        <v>0.9914137342631111</v>
       </c>
       <c r="S21">
-        <v>0.9841972903955454</v>
+        <v>0.9910330020663629</v>
       </c>
       <c r="T21">
-        <v>0.996698559388667</v>
+        <v>0.9990407046238504</v>
       </c>
       <c r="U21">
-        <v>0.9913952299403848</v>
+        <v>0.9966519727314627</v>
       </c>
       <c r="V21">
-        <v>0.9902485415308344</v>
+        <v>0.9962291889005441</v>
       </c>
       <c r="W21">
-        <v>0.9888455610941306</v>
+        <v>0.9958627895457421</v>
       </c>
       <c r="X21">
-        <v>0.9866504411874103</v>
+        <v>0.9951993218482899</v>
       </c>
       <c r="Y21">
-        <v>0.9739677499486911</v>
+        <v>0.9927081336842982</v>
       </c>
       <c r="Z21">
-        <v>0.9646710570950312</v>
+        <v>0.9923982441971227</v>
       </c>
       <c r="AA21">
-        <v>0.9863016822145331</v>
+        <v>0.9951719822394437</v>
       </c>
       <c r="AB21">
-        <v>0.9825469773094397</v>
+        <v>0.9938468592968938</v>
       </c>
       <c r="AC21">
-        <v>0.9667015130154392</v>
+        <v>0.9892779512754196</v>
       </c>
       <c r="AD21">
-        <v>0.9551232368799552</v>
+        <v>0.9863755305382996</v>
       </c>
       <c r="AE21">
-        <v>0.9493934581227437</v>
+        <v>0.9851342453619312</v>
       </c>
       <c r="AF21">
-        <v>0.9453610263200778</v>
+        <v>0.9836050961244256</v>
       </c>
       <c r="AG21">
-        <v>0.9444739751180152</v>
+        <v>0.9834980324440613</v>
       </c>
       <c r="AH21">
-        <v>0.9441994123822716</v>
+        <v>0.9834988515373787</v>
       </c>
     </row>
     <row r="22" spans="1:34">
@@ -2561,100 +2561,100 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>0.9984175689555534</v>
+        <v>0.9993754183567121</v>
       </c>
       <c r="D22">
-        <v>0.993258319374122</v>
+        <v>0.9975448049064685</v>
       </c>
       <c r="E22">
-        <v>0.9959215503072646</v>
+        <v>0.9985850501044286</v>
       </c>
       <c r="F22">
-        <v>0.9999999999999997</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G22">
-        <v>0.9890770014508669</v>
+        <v>0.9961887241175601</v>
       </c>
       <c r="H22">
-        <v>0.9977141127015308</v>
+        <v>1.000312005980476</v>
       </c>
       <c r="I22">
-        <v>0.9851551955053184</v>
+        <v>0.9949578154938605</v>
       </c>
       <c r="J22">
-        <v>0.9910921376126171</v>
+        <v>0.9972589632884225</v>
       </c>
       <c r="K22">
-        <v>0.999196618823489</v>
+        <v>1.000009665299512</v>
       </c>
       <c r="L22">
-        <v>0.9994119663230443</v>
+        <v>0.9999587612068068</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="N22">
-        <v>0.9924663721806065</v>
+        <v>0.9959295383688512</v>
       </c>
       <c r="O22">
-        <v>0.9892021151063739</v>
+        <v>0.9948074213152688</v>
       </c>
       <c r="P22">
-        <v>0.9878973269218967</v>
+        <v>0.9937852065846687</v>
       </c>
       <c r="Q22">
-        <v>0.9866323260860446</v>
+        <v>0.9927512120136277</v>
       </c>
       <c r="R22">
-        <v>0.984759608627942</v>
+        <v>0.991413734263107</v>
       </c>
       <c r="S22">
-        <v>0.9841972903955446</v>
+        <v>0.9910330020663587</v>
       </c>
       <c r="T22">
-        <v>0.9966982409499209</v>
+        <v>0.9990405730539186</v>
       </c>
       <c r="U22">
-        <v>0.9913949097713508</v>
+        <v>0.9966518408414927</v>
       </c>
       <c r="V22">
-        <v>0.9902482209875926</v>
+        <v>0.9962290569538973</v>
       </c>
       <c r="W22">
-        <v>0.9888452400938974</v>
+        <v>0.9958626575501112</v>
       </c>
       <c r="X22">
-        <v>0.986649220469161</v>
+        <v>0.9951988240689736</v>
       </c>
       <c r="Y22">
-        <v>0.9739665127550887</v>
+        <v>0.9927076346472083</v>
       </c>
       <c r="Z22">
-        <v>0.9646698078208716</v>
+        <v>0.9923977450030232</v>
       </c>
       <c r="AA22">
-        <v>0.9863016822145326</v>
+        <v>0.9951719822394447</v>
       </c>
       <c r="AB22">
-        <v>0.9825469773094393</v>
+        <v>0.9938468592968943</v>
       </c>
       <c r="AC22">
-        <v>0.9667015130154393</v>
+        <v>0.9892779512754202</v>
       </c>
       <c r="AD22">
-        <v>0.9551232368799556</v>
+        <v>0.9863755305382998</v>
       </c>
       <c r="AE22">
-        <v>0.9493934581227442</v>
+        <v>0.9851342453619312</v>
       </c>
       <c r="AF22">
-        <v>0.9453610263200788</v>
+        <v>0.9836050961244264</v>
       </c>
       <c r="AG22">
-        <v>0.9444739751180161</v>
+        <v>0.983498032444062</v>
       </c>
       <c r="AH22">
-        <v>0.9441994123822728</v>
+        <v>0.9834988515373793</v>
       </c>
     </row>
     <row r="23" spans="1:34">
@@ -2665,100 +2665,100 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>0.998407614994546</v>
+        <v>0.9993669903183657</v>
       </c>
       <c r="D23">
-        <v>0.9932140232377862</v>
+        <v>0.9975120024453559</v>
       </c>
       <c r="E23">
-        <v>0.9958932632706289</v>
+        <v>0.9985647697967405</v>
       </c>
       <c r="F23">
-        <v>0.9999999999999996</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0.9890439453692168</v>
+        <v>0.9961451170825667</v>
       </c>
       <c r="H23">
-        <v>0.9977217345019732</v>
+        <v>1.000319677284654</v>
       </c>
       <c r="I23">
-        <v>0.9850975193568997</v>
+        <v>0.9948944800622229</v>
       </c>
       <c r="J23">
-        <v>0.9910529912677335</v>
+        <v>0.9972239211409963</v>
       </c>
       <c r="K23">
-        <v>0.9991938402498096</v>
+        <v>1.000009702349428</v>
       </c>
       <c r="L23">
-        <v>0.9994099883293044</v>
+        <v>0.9999582182086911</v>
       </c>
       <c r="M23">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="N23">
-        <v>0.9924316250688084</v>
+        <v>0.9958849483268954</v>
       </c>
       <c r="O23">
-        <v>0.9891544716983585</v>
+        <v>0.9947503802341638</v>
       </c>
       <c r="P23">
-        <v>0.9878496195877683</v>
+        <v>0.9937168770743714</v>
       </c>
       <c r="Q23">
-        <v>0.986584556857885</v>
+        <v>0.9926714835156333</v>
       </c>
       <c r="R23">
-        <v>0.9847117474624593</v>
+        <v>0.9913192261059883</v>
       </c>
       <c r="S23">
-        <v>0.984149401780358</v>
+        <v>0.9909343067867363</v>
       </c>
       <c r="T23">
-        <v>0.9966861076464693</v>
+        <v>0.9990282712440455</v>
       </c>
       <c r="U23">
-        <v>0.9913644048266697</v>
+        <v>0.9966133181650576</v>
       </c>
       <c r="V23">
-        <v>0.9902128482068602</v>
+        <v>0.9961858920951231</v>
       </c>
       <c r="W23">
-        <v>0.9888014810339204</v>
+        <v>0.9958154751485263</v>
       </c>
       <c r="X23">
-        <v>0.9865705214162215</v>
+        <v>0.9951402868672784</v>
       </c>
       <c r="Y23">
-        <v>0.9738195916648973</v>
+        <v>0.9926217413179107</v>
       </c>
       <c r="Z23">
-        <v>0.9644559367730784</v>
+        <v>0.9923084427062377</v>
       </c>
       <c r="AA23">
-        <v>0.9862582217224438</v>
+        <v>0.9951171026447631</v>
       </c>
       <c r="AB23">
-        <v>0.9824889535467817</v>
+        <v>0.9937772817016823</v>
       </c>
       <c r="AC23">
-        <v>0.966588493861222</v>
+        <v>0.9891575464076994</v>
       </c>
       <c r="AD23">
-        <v>0.9549686837063339</v>
+        <v>0.9862228946945123</v>
       </c>
       <c r="AE23">
-        <v>0.9492130324844058</v>
+        <v>0.9849678499760796</v>
       </c>
       <c r="AF23">
-        <v>0.9451798233763065</v>
+        <v>0.9834216934318261</v>
       </c>
       <c r="AG23">
-        <v>0.9442926011225441</v>
+        <v>0.9833134267401785</v>
       </c>
       <c r="AH23">
-        <v>0.9440179853145176</v>
+        <v>0.9833142456797496</v>
       </c>
     </row>
     <row r="24" spans="1:34">
@@ -2769,100 +2769,100 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>0.9984625591440979</v>
+        <v>0.999415292638814</v>
       </c>
       <c r="D24">
-        <v>0.9934615251940185</v>
+        <v>0.9977002796976644</v>
       </c>
       <c r="E24">
-        <v>0.9960480692649848</v>
+        <v>0.998679504446481</v>
       </c>
       <c r="F24">
-        <v>0.9999999999999998</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G24">
-        <v>0.9892412089282154</v>
+        <v>0.9964054442343785</v>
       </c>
       <c r="H24">
-        <v>0.9976756364740855</v>
+        <v>1.00027323087745</v>
       </c>
       <c r="I24">
-        <v>0.98544128540551</v>
+        <v>0.995271654742785</v>
       </c>
       <c r="J24">
-        <v>0.9912862482138721</v>
+        <v>0.9974321674743419</v>
       </c>
       <c r="K24">
-        <v>0.9992101375232098</v>
+        <v>1.000009015564735</v>
       </c>
       <c r="L24">
-        <v>0.9994215965627655</v>
+        <v>0.9999611535462243</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="N24">
-        <v>0.9926400550680791</v>
+        <v>0.9961523849394331</v>
       </c>
       <c r="O24">
-        <v>0.9894402562671258</v>
+        <v>0.9950924756626278</v>
       </c>
       <c r="P24">
-        <v>0.9881357875183563</v>
+        <v>0.9941266655035952</v>
       </c>
       <c r="Q24">
-        <v>0.986871095963802</v>
+        <v>0.9931496286612315</v>
       </c>
       <c r="R24">
-        <v>0.98499883791161</v>
+        <v>0.991885998735991</v>
       </c>
       <c r="S24">
-        <v>0.9844366568438319</v>
+        <v>0.9915261893775446</v>
       </c>
       <c r="T24">
-        <v>0.9967541000044458</v>
+        <v>0.9990997842050376</v>
       </c>
       <c r="U24">
-        <v>0.9915425648638764</v>
+        <v>0.9968421053224799</v>
       </c>
       <c r="V24">
-        <v>0.9904202008332542</v>
+        <v>0.9964425241934268</v>
       </c>
       <c r="W24">
-        <v>0.9890591315702238</v>
+        <v>0.9960962055380674</v>
       </c>
       <c r="X24">
-        <v>0.9870240009405394</v>
+        <v>0.9954828852734542</v>
       </c>
       <c r="Y24">
-        <v>0.9746815685494334</v>
+        <v>0.99312837708404</v>
       </c>
       <c r="Z24">
-        <v>0.9657189379017689</v>
+        <v>0.9928355203732734</v>
       </c>
       <c r="AA24">
-        <v>0.9865178315241597</v>
+        <v>0.995444999447241</v>
       </c>
       <c r="AB24">
-        <v>0.9828358319702257</v>
+        <v>0.9941932778814321</v>
       </c>
       <c r="AC24">
-        <v>0.9672648979391698</v>
+        <v>0.989878171716196</v>
       </c>
       <c r="AD24">
-        <v>0.9558939973790256</v>
+        <v>0.9871367110425561</v>
       </c>
       <c r="AE24">
-        <v>0.9502934182950818</v>
+        <v>0.985964143461496</v>
       </c>
       <c r="AF24">
-        <v>0.946264859209456</v>
+        <v>0.9845199277676863</v>
       </c>
       <c r="AG24">
-        <v>0.9453786602265214</v>
+        <v>0.9844188721145124</v>
       </c>
       <c r="AH24">
-        <v>0.9451043619093336</v>
+        <v>0.9844196919747387</v>
       </c>
     </row>
     <row r="25" spans="1:34">
@@ -2873,100 +2873,100 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>0.998594300898083</v>
+        <v>0.9995308478516902</v>
       </c>
       <c r="D25">
-        <v>0.9940583602449113</v>
+        <v>0.9981515336191102</v>
       </c>
       <c r="E25">
-        <v>0.9964180238583215</v>
+        <v>0.9989507772675699</v>
       </c>
       <c r="F25">
-        <v>0.9999999999999998</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>0.9897233766624712</v>
+        <v>0.9970428123063386</v>
       </c>
       <c r="H25">
-        <v>0.9975566040636613</v>
+        <v>1.000152810417148</v>
       </c>
       <c r="I25">
-        <v>0.9862773445441821</v>
+        <v>0.9961856931648524</v>
       </c>
       <c r="J25">
-        <v>0.9918528713368183</v>
+        <v>0.9979323603819238</v>
       </c>
       <c r="K25">
-        <v>0.9992470707374689</v>
+        <v>1.000002575207299</v>
       </c>
       <c r="L25">
-        <v>0.9994479726502919</v>
+        <v>0.9999652111196597</v>
       </c>
       <c r="M25">
-        <v>1</v>
+        <v>0.9999999999999997</v>
       </c>
       <c r="N25">
-        <v>0.993160578104379</v>
+        <v>0.9968198918109967</v>
       </c>
       <c r="O25">
-        <v>0.9901539225680862</v>
+        <v>0.9959461336011466</v>
       </c>
       <c r="P25">
-        <v>0.9888504101829915</v>
+        <v>0.9951491629554735</v>
       </c>
       <c r="Q25">
-        <v>0.9875866445887822</v>
+        <v>0.9943426287545627</v>
       </c>
       <c r="R25">
-        <v>0.9857157619546909</v>
+        <v>0.9933000397853339</v>
       </c>
       <c r="S25">
-        <v>0.9851539915440294</v>
+        <v>0.9930028717317259</v>
       </c>
       <c r="T25">
-        <v>0.9969182513291642</v>
+        <v>0.9992730381793316</v>
       </c>
       <c r="U25">
-        <v>0.9919817281484107</v>
+        <v>0.9974080582778304</v>
       </c>
       <c r="V25">
-        <v>0.990932247340556</v>
+        <v>0.9970780125631948</v>
       </c>
       <c r="W25">
-        <v>0.9896967806514004</v>
+        <v>0.9967918739899317</v>
       </c>
       <c r="X25">
-        <v>0.98813240983557</v>
+        <v>0.996319204753685</v>
       </c>
       <c r="Y25">
-        <v>0.9768048551066427</v>
+        <v>0.9943739373634061</v>
       </c>
       <c r="Z25">
-        <v>0.9688394661302226</v>
+        <v>0.9941320842500941</v>
       </c>
       <c r="AA25">
-        <v>0.9871550321003815</v>
+        <v>0.9962506093635946</v>
       </c>
       <c r="AB25">
-        <v>0.9836900519121148</v>
+        <v>0.9952182159886492</v>
       </c>
       <c r="AC25">
-        <v>0.9689382967398689</v>
+        <v>0.99166120956044</v>
       </c>
       <c r="AD25">
-        <v>0.958186615818716</v>
+        <v>0.9894007048009859</v>
       </c>
       <c r="AE25">
-        <v>0.9529720304524318</v>
+        <v>0.9884334988132158</v>
       </c>
       <c r="AF25">
-        <v>0.9489549541058447</v>
+        <v>0.9872430666498518</v>
       </c>
       <c r="AG25">
-        <v>0.9480712819784345</v>
+        <v>0.987159965662173</v>
       </c>
       <c r="AH25">
-        <v>0.9477977676719307</v>
+        <v>0.9871607878052827</v>
       </c>
     </row>
   </sheetData>

</xml_diff>